<commit_message>
Updated cheat-sheet with planet colors
</commit_message>
<xml_diff>
--- a/Room Setup/HelioRoom Calculator.xlsx
+++ b/Room Setup/HelioRoom Calculator.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Room radius (ft)</t>
   </si>
@@ -73,6 +73,36 @@
   </si>
   <si>
     <t>Ratio</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Pink</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Gray</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Purple</t>
   </si>
 </sst>
 </file>
@@ -80,7 +110,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -138,8 +168,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -151,14 +183,16 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -488,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -503,7 +537,7 @@
     <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,18 +547,21 @@
       <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -534,30 +571,36 @@
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2">
         <v>88</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>1</v>
       </c>
-      <c r="H2" s="5">
-        <f>F2/E2</f>
+      <c r="I2" s="5">
+        <f>G2/F2</f>
         <v>1.1363636363636364E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3">
         <v>224.7</v>
       </c>
-      <c r="F3" s="6">
-        <f>E3*H$2</f>
+      <c r="G3" s="6">
+        <f>F3*I$2</f>
         <v>2.5534090909090907</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -568,15 +611,18 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4">
         <v>365.2</v>
       </c>
-      <c r="F4" s="6">
-        <f t="shared" ref="F4:F10" si="0">E4*H$2</f>
+      <c r="G4" s="6">
+        <f>F4*I$2</f>
         <v>4.1500000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -587,27 +633,33 @@
       <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5">
         <v>687</v>
       </c>
-      <c r="F5" s="6">
-        <f t="shared" si="0"/>
+      <c r="G5" s="6">
+        <f>F5*I$2</f>
         <v>7.8068181818181817</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6">
         <v>4332</v>
       </c>
-      <c r="F6" s="6">
-        <f t="shared" si="0"/>
+      <c r="G6" s="6">
+        <f>F6*I$2</f>
         <v>49.227272727272727</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -618,47 +670,59 @@
       <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7">
         <v>10760</v>
       </c>
-      <c r="F7" s="6">
-        <f t="shared" si="0"/>
+      <c r="G7" s="6">
+        <f>F7*I$2</f>
         <v>122.27272727272728</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8">
         <v>30700</v>
       </c>
-      <c r="F8" s="6">
-        <f t="shared" si="0"/>
+      <c r="G8" s="6">
+        <f>F8*I$2</f>
         <v>348.86363636363637</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="D9" t="s">
         <v>12</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9">
         <v>60200</v>
       </c>
-      <c r="F9" s="6">
-        <f t="shared" si="0"/>
+      <c r="G9" s="6">
+        <f>F9*I$2</f>
         <v>684.09090909090912</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10">
         <v>90600</v>
       </c>
-      <c r="F10" s="6">
-        <f t="shared" si="0"/>
+      <c r="G10" s="6">
+        <f>F10*I$2</f>
         <v>1029.5454545454545</v>
       </c>
     </row>

</xml_diff>